<commit_message>
Git test diff config
</commit_message>
<xml_diff>
--- a/OIP_Kyrgyzstan(update) (1).xlsx
+++ b/OIP_Kyrgyzstan(update) (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/58f519ef3195455a/Документы/GitHub/zerkalo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{B7D0B2CC-6386-4515-833A-CE734F5488B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F56DDE4-DAA3-4091-91B7-F94DEBEA5C50}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{B7D0B2CC-6386-4515-833A-CE734F5488B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{096464AD-5699-43F8-9E10-EC0D04E6FD21}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3216" uniqueCount="1194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3217" uniqueCount="1195">
   <si>
     <t>type</t>
   </si>
@@ -3670,6 +3670,9 @@
   </si>
   <si>
     <t>Begin time</t>
+  </si>
+  <si>
+    <t>it was start time before the change</t>
   </si>
 </sst>
 </file>
@@ -5154,7 +5157,7 @@
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5234,6 +5237,9 @@
       </c>
       <c r="C2" s="10" t="s">
         <v>1193</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>1194</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>255</v>
@@ -14821,7 +14827,7 @@
       </c>
       <c r="W2">
         <f ca="1">RAND()</f>
-        <v>0.94777086601957949</v>
+        <v>0.3071448025917829</v>
       </c>
       <c r="Z2" t="s">
         <v>110</v>
@@ -14908,7 +14914,7 @@
       </c>
       <c r="W3">
         <f t="shared" ref="W3:W19" ca="1" si="1">RAND()</f>
-        <v>0.59831855466803718</v>
+        <v>0.21723671122256527</v>
       </c>
       <c r="Z3" t="s">
         <v>102</v>
@@ -15001,7 +15007,7 @@
       </c>
       <c r="W4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.41934728283360156</v>
+        <v>0.27020451050006555</v>
       </c>
       <c r="Z4" t="s">
         <v>103</v>
@@ -15094,7 +15100,7 @@
       </c>
       <c r="W5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.66860938873307163</v>
+        <v>0.74601199692843356</v>
       </c>
       <c r="Z5" t="s">
         <v>111</v>
@@ -15182,7 +15188,7 @@
       </c>
       <c r="W6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.33193829071857595</v>
+        <v>0.58803987071884256</v>
       </c>
       <c r="Z6" t="s">
         <v>104</v>
@@ -15245,7 +15251,7 @@
       </c>
       <c r="W7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.50520689412434472</v>
+        <v>0.2350352728752193</v>
       </c>
       <c r="Z7" t="s">
         <v>108</v>
@@ -15308,7 +15314,7 @@
       </c>
       <c r="W8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.46747483905361986</v>
+        <v>0.36030735016153514</v>
       </c>
       <c r="Z8" t="s">
         <v>114</v>
@@ -15367,7 +15373,7 @@
       </c>
       <c r="W9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.58174286036455092</v>
+        <v>0.168795764530426</v>
       </c>
       <c r="Z9" t="s">
         <v>109</v>
@@ -15436,7 +15442,7 @@
       </c>
       <c r="W10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.69848550620487937</v>
+        <v>0.16403244001010198</v>
       </c>
       <c r="Z10" t="s">
         <v>106</v>
@@ -15500,7 +15506,7 @@
       </c>
       <c r="W11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.68585581170067933</v>
+        <v>0.63852230178481761</v>
       </c>
       <c r="Z11" t="s">
         <v>105</v>
@@ -15569,7 +15575,7 @@
       </c>
       <c r="W12">
         <f t="shared" ca="1" si="1"/>
-        <v>0.94387835945006171</v>
+        <v>0.93466990604408973</v>
       </c>
       <c r="Z12" t="s">
         <v>112</v>
@@ -15633,7 +15639,7 @@
       </c>
       <c r="W13">
         <f t="shared" ca="1" si="1"/>
-        <v>0.33277065701857922</v>
+        <v>0.24904290059415191</v>
       </c>
       <c r="Z13" t="s">
         <v>107</v>
@@ -15698,7 +15704,7 @@
       </c>
       <c r="W14">
         <f t="shared" ca="1" si="1"/>
-        <v>0.1172957036344443</v>
+        <v>0.57545360422819614</v>
       </c>
       <c r="Z14" t="s">
         <v>113</v>
@@ -15762,7 +15768,7 @@
       </c>
       <c r="W15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.38595798809184612</v>
+        <v>0.9860657116574042</v>
       </c>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.3">
@@ -15790,7 +15796,7 @@
       </c>
       <c r="W16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.96872312390896687</v>
+        <v>0.60835564486886828</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.3">
@@ -15818,7 +15824,7 @@
       </c>
       <c r="W17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.32970306798662119</v>
+        <v>0.60535045724391212</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.3">
@@ -15846,7 +15852,7 @@
       </c>
       <c r="W18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.98868114095026816</v>
+        <v>0.58531049597204565</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.3">
@@ -15874,7 +15880,7 @@
       </c>
       <c r="W19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.72303959662422501</v>
+        <v>0.58174369207790111</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.3">

</xml_diff>